<commit_message>
seek for best clustering state
</commit_message>
<xml_diff>
--- a/Earliness prediction.xlsx
+++ b/Earliness prediction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Desktop\TFE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\data\KMedoids-clustering-BPIC-2017 final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{B58C97FA-2B3A-47D7-9830-9F018F7D77B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7965FA71-9495-45E9-BF1C-08028E5E7354}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5925" yWindow="1575" windowWidth="22575" windowHeight="13380"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -104,7 +104,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -205,7 +205,7 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -279,37 +279,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.18999999999999997</c:v>
+                  <c:v>0.56999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.21333333333333335</c:v>
+                  <c:v>0.64</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25666666666666665</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.26333333333333336</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.27999999999999997</c:v>
+                  <c:v>0.83999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.31</c:v>
+                  <c:v>0.92999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.31666666666666665</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.32333333333333331</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.32333333333333331</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.32333333333333331</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.32666666666666666</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -392,37 +392,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.18333333333333335</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22666666666666668</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.28999999999999998</c:v>
+                  <c:v>0.86999999999999988</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.29666666666666669</c:v>
+                  <c:v>0.89000000000000012</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3066666666666667</c:v>
+                  <c:v>0.92000000000000015</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.32333333333333331</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.32666666666666666</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.33</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.33</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -505,37 +505,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.18333333333333335</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18333333333333335</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22666666666666668</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.23666666666666666</c:v>
+                  <c:v>0.71</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25666666666666665</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.29333333333333333</c:v>
+                  <c:v>0.88</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.30333333333333334</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.31</c:v>
+                  <c:v>0.92999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.3133333333333333</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.3133333333333333</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.3133333333333333</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -555,7 +555,6 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
         <c:axId val="605344383"/>
         <c:axId val="715984831"/>
       </c:barChart>
@@ -873,37 +872,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.55666666666666664</c:v>
+                  <c:v>1.6700000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.62333333333333341</c:v>
+                  <c:v>1.87</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.77333333333333332</c:v>
+                  <c:v>2.3199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.79666666666666675</c:v>
+                  <c:v>2.39</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.84333333333333327</c:v>
+                  <c:v>2.5300000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.92666666666666664</c:v>
+                  <c:v>2.78</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.94666666666666666</c:v>
+                  <c:v>2.84</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.96333333333333337</c:v>
+                  <c:v>2.8899999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.96666666666666656</c:v>
+                  <c:v>2.9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.97</c:v>
+                  <c:v>2.91</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.97333333333333316</c:v>
+                  <c:v>2.92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1158,7 +1157,7 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
@@ -1232,37 +1231,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.16666666666666666</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.21666666666666667</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.27333333333333332</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.3133333333333333</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.32333333333333331</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.32666666666666666</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.33</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.33</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.33</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1345,37 +1344,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.17</c:v>
+                  <c:v>0.51</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18999999999999997</c:v>
+                  <c:v>0.56999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.27999999999999997</c:v>
+                  <c:v>0.83999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.29666666666666669</c:v>
+                  <c:v>0.89000000000000012</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.3</c:v>
+                  <c:v>0.89999999999999991</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3066666666666667</c:v>
+                  <c:v>0.92000000000000015</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.31</c:v>
+                  <c:v>0.92999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.3133333333333333</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.3133333333333333</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1458,37 +1457,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.16666666666666666</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18000000000000002</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19333333333333333</c:v>
+                  <c:v>0.57999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25666666666666665</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3</c:v>
+                  <c:v>0.89999999999999991</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3133333333333333</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.31666666666666665</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.32333333333333331</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.32333333333333331</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.32666666666666666</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.32666666666666666</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1508,7 +1507,6 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
         <c:axId val="715021935"/>
         <c:axId val="793739711"/>
         <c:extLst>
@@ -1920,37 +1918,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.5033333333333333</c:v>
+                  <c:v>1.51</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.58666666666666667</c:v>
+                  <c:v>1.76</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.68666666666666665</c:v>
+                  <c:v>2.06</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.81999999999999984</c:v>
+                  <c:v>2.46</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.89999999999999991</c:v>
+                  <c:v>2.6999999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.93333333333333335</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.94333333333333336</c:v>
+                  <c:v>2.83</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.96</c:v>
+                  <c:v>2.88</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.96333333333333337</c:v>
+                  <c:v>2.8899999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.97</c:v>
+                  <c:v>2.91</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.97333333333333327</c:v>
+                  <c:v>2.92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2081,7 +2079,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$29</c15:sqref>
@@ -2110,7 +2108,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$27:$L$27</c15:sqref>
@@ -2157,7 +2155,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$29:$L$29</c15:sqref>
@@ -2168,43 +2166,43 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="11"/>
                       <c:pt idx="0">
-                        <c:v>0.16666666666666666</c:v>
+                        <c:v>0.5</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.21666666666666667</c:v>
+                        <c:v>0.65</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.27333333333333332</c:v>
+                        <c:v>0.82</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.3133333333333333</c:v>
+                        <c:v>0.94</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0.32</c:v>
+                        <c:v>0.96</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>0.32333333333333331</c:v>
+                        <c:v>0.97</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.32666666666666666</c:v>
+                        <c:v>0.98</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>0.33</c:v>
+                        <c:v>0.99</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>0.33</c:v>
+                        <c:v>0.99</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0.33</c:v>
+                        <c:v>0.99</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>0.33333333333333331</c:v>
+                        <c:v>1</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-3658-4E8A-BA1C-DFF212288065}"/>
                   </c:ext>
@@ -2217,7 +2215,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$30</c15:sqref>
@@ -2246,7 +2244,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$27:$L$27</c15:sqref>
@@ -2293,7 +2291,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$30:$L$30</c15:sqref>
@@ -2304,43 +2302,43 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="11"/>
                       <c:pt idx="0">
-                        <c:v>0.17</c:v>
+                        <c:v>0.51</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.18999999999999997</c:v>
+                        <c:v>0.56999999999999995</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.22</c:v>
+                        <c:v>0.66</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.25</c:v>
+                        <c:v>0.75</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0.27999999999999997</c:v>
+                        <c:v>0.83999999999999986</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>0.29666666666666669</c:v>
+                        <c:v>0.89000000000000012</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.3</c:v>
+                        <c:v>0.89999999999999991</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>0.3066666666666667</c:v>
+                        <c:v>0.92000000000000015</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>0.31</c:v>
+                        <c:v>0.92999999999999994</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0.3133333333333333</c:v>
+                        <c:v>0.94</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>0.3133333333333333</c:v>
+                        <c:v>0.94</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-3658-4E8A-BA1C-DFF212288065}"/>
                   </c:ext>
@@ -2353,7 +2351,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$31</c15:sqref>
@@ -2382,7 +2380,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$27:$L$27</c15:sqref>
@@ -2429,7 +2427,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$31:$L$31</c15:sqref>
@@ -2440,43 +2438,43 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="11"/>
                       <c:pt idx="0">
-                        <c:v>0.16666666666666666</c:v>
+                        <c:v>0.5</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.18000000000000002</c:v>
+                        <c:v>0.54</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.19333333333333333</c:v>
+                        <c:v>0.57999999999999996</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.25666666666666665</c:v>
+                        <c:v>0.77</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0.3</c:v>
+                        <c:v>0.89999999999999991</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>0.3133333333333333</c:v>
+                        <c:v>0.94</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.31666666666666665</c:v>
+                        <c:v>0.95</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>0.32333333333333331</c:v>
+                        <c:v>0.97</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>0.32333333333333331</c:v>
+                        <c:v>0.97</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0.32666666666666666</c:v>
+                        <c:v>0.98</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>0.32666666666666666</c:v>
+                        <c:v>0.98</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-3658-4E8A-BA1C-DFF212288065}"/>
                   </c:ext>
@@ -2489,7 +2487,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$32</c15:sqref>
@@ -2515,7 +2513,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$27:$L$27</c15:sqref>
@@ -2562,7 +2560,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$32:$L$32</c15:sqref>
@@ -2576,7 +2574,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-3658-4E8A-BA1C-DFF212288065}"/>
                   </c:ext>
@@ -2848,7 +2846,7 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -2874,6 +2872,47 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$54:$L$54</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>all</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$56:$L$56</c:f>
@@ -2881,37 +2920,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.19999999999999998</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.29333333333333333</c:v>
+                  <c:v>0.88</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.31</c:v>
+                  <c:v>0.92999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.32333333333333331</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.32666666666666666</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.33</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.33</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.33</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.33</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2946,6 +2985,47 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$54:$L$54</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>all</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$57:$L$57</c:f>
@@ -2953,37 +3033,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.19999999999999998</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.21333333333333335</c:v>
+                  <c:v>0.64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.24666666666666667</c:v>
+                  <c:v>0.74</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.26</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.27333333333333332</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.27999999999999997</c:v>
+                  <c:v>0.83999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.28333333333333333</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.28333333333333333</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.28666666666666668</c:v>
+                  <c:v>0.8600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.28666666666666668</c:v>
+                  <c:v>0.8600000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3018,6 +3098,47 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$54:$L$54</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>all</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$58:$L$58</c:f>
@@ -3025,37 +3146,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.19999999999999998</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25666666666666665</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27333333333333332</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.29333333333333333</c:v>
+                  <c:v>0.88</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.30333333333333334</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.31</c:v>
+                  <c:v>0.92999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3133333333333333</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.3133333333333333</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.3133333333333333</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.31666666666666665</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3075,7 +3196,6 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
         <c:axId val="613136047"/>
         <c:axId val="791631247"/>
       </c:barChart>
@@ -3386,37 +3506,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.6</c:v>
+                  <c:v>1.7999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66</c:v>
+                  <c:v>1.98</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.76333333333333342</c:v>
+                  <c:v>2.29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.83</c:v>
+                  <c:v>2.4899999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.87333333333333341</c:v>
+                  <c:v>2.62</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.91666666666666674</c:v>
+                  <c:v>2.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.92666666666666653</c:v>
+                  <c:v>2.78</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.92666666666666653</c:v>
+                  <c:v>2.78</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.92999999999999994</c:v>
+                  <c:v>2.79</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.93333333333333335</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3544,6 +3664,703 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="848871279"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>all</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$L$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.83999999999999986</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.92999999999999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FE65-4014-B84A-CCE5B0CB31F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>all</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.86999999999999988</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89000000000000012</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.92000000000000015</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FE65-4014-B84A-CCE5B0CB31F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>all</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$L$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.92999999999999994</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FE65-4014-B84A-CCE5B0CB31F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="761153855"/>
+        <c:axId val="765040655"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$1:$L$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="11"/>
+                      <c:pt idx="0">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>all</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$2:$L$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="11"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-FE65-4014-B84A-CCE5B0CB31F8}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="761153855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="765040655"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="765040655"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="761153855"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3863,6 +4680,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -6411,6 +7268,522 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7144,6 +8517,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BDDA088-1312-4AB2-A9C7-89F9EAB2D9E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7443,11 +8852,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7502,37 +8911,37 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>0.18999999999999997</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="C3">
-        <v>0.21333333333333335</v>
+        <v>0.64</v>
       </c>
       <c r="D3">
-        <v>0.25666666666666665</v>
+        <v>0.77</v>
       </c>
       <c r="E3">
-        <v>0.26333333333333336</v>
+        <v>0.79</v>
       </c>
       <c r="F3">
-        <v>0.27999999999999997</v>
+        <v>0.83999999999999986</v>
       </c>
       <c r="G3">
-        <v>0.31</v>
+        <v>0.92999999999999994</v>
       </c>
       <c r="H3">
-        <v>0.31666666666666665</v>
+        <v>0.95</v>
       </c>
       <c r="I3">
-        <v>0.32333333333333331</v>
+        <v>0.97</v>
       </c>
       <c r="J3">
-        <v>0.32333333333333331</v>
+        <v>0.97</v>
       </c>
       <c r="K3">
-        <v>0.32333333333333331</v>
+        <v>0.97</v>
       </c>
       <c r="L3">
-        <v>0.32666666666666666</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -7540,37 +8949,40 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0.18333333333333335</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C4">
-        <v>0.22666666666666668</v>
+        <v>0.68</v>
       </c>
       <c r="D4">
-        <v>0.28999999999999998</v>
+        <v>0.86999999999999988</v>
       </c>
       <c r="E4">
-        <v>0.29666666666666669</v>
+        <v>0.89000000000000012</v>
       </c>
       <c r="F4">
-        <v>0.3066666666666667</v>
+        <v>0.92000000000000015</v>
       </c>
       <c r="G4">
-        <v>0.32333333333333331</v>
+        <v>0.97</v>
       </c>
       <c r="H4">
-        <v>0.32666666666666666</v>
+        <v>0.98</v>
       </c>
       <c r="I4">
-        <v>0.33</v>
+        <v>0.99</v>
       </c>
       <c r="J4">
-        <v>0.33</v>
+        <v>0.99</v>
       </c>
       <c r="K4">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>0.33333333333333331</v>
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -7578,37 +8990,37 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>0.18333333333333335</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C5">
-        <v>0.18333333333333335</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D5">
-        <v>0.22666666666666668</v>
+        <v>0.68</v>
       </c>
       <c r="E5">
-        <v>0.23666666666666666</v>
+        <v>0.71</v>
       </c>
       <c r="F5">
-        <v>0.25666666666666665</v>
+        <v>0.77</v>
       </c>
       <c r="G5">
-        <v>0.29333333333333333</v>
+        <v>0.88</v>
       </c>
       <c r="H5">
-        <v>0.30333333333333334</v>
+        <v>0.91</v>
       </c>
       <c r="I5">
-        <v>0.31</v>
+        <v>0.92999999999999994</v>
       </c>
       <c r="J5">
-        <v>0.3133333333333333</v>
+        <v>0.94</v>
       </c>
       <c r="K5">
-        <v>0.3133333333333333</v>
+        <v>0.94</v>
       </c>
       <c r="L5">
-        <v>0.3133333333333333</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -7617,47 +9029,47 @@
       </c>
       <c r="B7">
         <f>SUM(B3:B5)</f>
-        <v>0.55666666666666664</v>
+        <v>1.6700000000000002</v>
       </c>
       <c r="C7">
         <f t="shared" ref="C7:L7" si="0">SUM(C3:C5)</f>
-        <v>0.62333333333333341</v>
+        <v>1.87</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.77333333333333332</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0.79666666666666675</v>
+        <v>2.39</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>0.84333333333333327</v>
+        <v>2.5300000000000002</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>0.92666666666666664</v>
+        <v>2.78</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>0.94666666666666666</v>
+        <v>2.84</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>0.96333333333333337</v>
+        <v>2.8899999999999997</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>0.96666666666666656</v>
+        <v>2.9</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>0.97</v>
+        <v>2.91</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>0.97333333333333316</v>
+        <v>2.92</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -7713,37 +9125,37 @@
         <v>1</v>
       </c>
       <c r="B29">
-        <v>0.16666666666666666</v>
+        <v>0.5</v>
       </c>
       <c r="C29">
-        <v>0.21666666666666667</v>
+        <v>0.65</v>
       </c>
       <c r="D29">
-        <v>0.27333333333333332</v>
+        <v>0.82</v>
       </c>
       <c r="E29">
-        <v>0.3133333333333333</v>
+        <v>0.94</v>
       </c>
       <c r="F29">
-        <v>0.32</v>
+        <v>0.96</v>
       </c>
       <c r="G29">
-        <v>0.32333333333333331</v>
+        <v>0.97</v>
       </c>
       <c r="H29">
-        <v>0.32666666666666666</v>
+        <v>0.98</v>
       </c>
       <c r="I29">
-        <v>0.33</v>
+        <v>0.99</v>
       </c>
       <c r="J29">
-        <v>0.33</v>
+        <v>0.99</v>
       </c>
       <c r="K29">
-        <v>0.33</v>
+        <v>0.99</v>
       </c>
       <c r="L29">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
@@ -7751,37 +9163,37 @@
         <v>2</v>
       </c>
       <c r="B30">
-        <v>0.17</v>
+        <v>0.51</v>
       </c>
       <c r="C30">
-        <v>0.18999999999999997</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="D30">
-        <v>0.22</v>
+        <v>0.66</v>
       </c>
       <c r="E30">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="F30">
-        <v>0.27999999999999997</v>
+        <v>0.83999999999999986</v>
       </c>
       <c r="G30">
-        <v>0.29666666666666669</v>
+        <v>0.89000000000000012</v>
       </c>
       <c r="H30">
-        <v>0.3</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="I30">
-        <v>0.3066666666666667</v>
+        <v>0.92000000000000015</v>
       </c>
       <c r="J30">
-        <v>0.31</v>
+        <v>0.92999999999999994</v>
       </c>
       <c r="K30">
-        <v>0.3133333333333333</v>
+        <v>0.94</v>
       </c>
       <c r="L30">
-        <v>0.3133333333333333</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
@@ -7789,37 +9201,37 @@
         <v>0</v>
       </c>
       <c r="B31">
-        <v>0.16666666666666666</v>
+        <v>0.5</v>
       </c>
       <c r="C31">
-        <v>0.18000000000000002</v>
+        <v>0.54</v>
       </c>
       <c r="D31">
-        <v>0.19333333333333333</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E31">
-        <v>0.25666666666666665</v>
+        <v>0.77</v>
       </c>
       <c r="F31">
-        <v>0.3</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="G31">
-        <v>0.3133333333333333</v>
+        <v>0.94</v>
       </c>
       <c r="H31">
-        <v>0.31666666666666665</v>
+        <v>0.95</v>
       </c>
       <c r="I31">
-        <v>0.32333333333333331</v>
+        <v>0.97</v>
       </c>
       <c r="J31">
-        <v>0.32333333333333331</v>
+        <v>0.97</v>
       </c>
       <c r="K31">
-        <v>0.32666666666666666</v>
+        <v>0.98</v>
       </c>
       <c r="L31">
-        <v>0.32666666666666666</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -7828,47 +9240,47 @@
       </c>
       <c r="B33">
         <f>SUM(B29:B31)</f>
-        <v>0.5033333333333333</v>
+        <v>1.51</v>
       </c>
       <c r="C33">
         <f t="shared" ref="C33:L33" si="1">SUM(C29:C31)</f>
-        <v>0.58666666666666667</v>
+        <v>1.76</v>
       </c>
       <c r="D33">
         <f t="shared" si="1"/>
-        <v>0.68666666666666665</v>
+        <v>2.06</v>
       </c>
       <c r="E33">
         <f t="shared" si="1"/>
-        <v>0.81999999999999984</v>
+        <v>2.46</v>
       </c>
       <c r="F33">
         <f t="shared" si="1"/>
-        <v>0.89999999999999991</v>
+        <v>2.6999999999999997</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
-        <v>0.93333333333333335</v>
+        <v>2.8</v>
       </c>
       <c r="H33">
         <f t="shared" si="1"/>
-        <v>0.94333333333333336</v>
+        <v>2.83</v>
       </c>
       <c r="I33">
         <f t="shared" si="1"/>
-        <v>0.96</v>
+        <v>2.88</v>
       </c>
       <c r="J33">
         <f t="shared" si="1"/>
-        <v>0.96333333333333337</v>
+        <v>2.8899999999999997</v>
       </c>
       <c r="K33">
         <f t="shared" si="1"/>
-        <v>0.97</v>
+        <v>2.91</v>
       </c>
       <c r="L33">
         <f t="shared" si="1"/>
-        <v>0.97333333333333327</v>
+        <v>2.92</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
@@ -7921,37 +9333,37 @@
         <v>1</v>
       </c>
       <c r="B56">
-        <v>0.19999999999999998</v>
+        <v>0.6</v>
       </c>
       <c r="C56">
-        <v>0.22</v>
+        <v>0.66</v>
       </c>
       <c r="D56">
-        <v>0.29333333333333333</v>
+        <v>0.88</v>
       </c>
       <c r="E56">
-        <v>0.31</v>
+        <v>0.92999999999999994</v>
       </c>
       <c r="F56">
-        <v>0.32</v>
+        <v>0.96</v>
       </c>
       <c r="G56">
-        <v>0.32333333333333331</v>
+        <v>0.97</v>
       </c>
       <c r="H56">
-        <v>0.32666666666666666</v>
+        <v>0.98</v>
       </c>
       <c r="I56">
-        <v>0.33</v>
+        <v>0.99</v>
       </c>
       <c r="J56">
-        <v>0.33</v>
+        <v>0.99</v>
       </c>
       <c r="K56">
-        <v>0.33</v>
+        <v>0.99</v>
       </c>
       <c r="L56">
-        <v>0.33</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
@@ -7959,37 +9371,37 @@
         <v>2</v>
       </c>
       <c r="B57">
-        <v>0.19999999999999998</v>
+        <v>0.6</v>
       </c>
       <c r="C57">
-        <v>0.22</v>
+        <v>0.66</v>
       </c>
       <c r="D57">
-        <v>0.21333333333333335</v>
+        <v>0.64</v>
       </c>
       <c r="E57">
-        <v>0.24666666666666667</v>
+        <v>0.74</v>
       </c>
       <c r="F57">
-        <v>0.26</v>
+        <v>0.78</v>
       </c>
       <c r="G57">
-        <v>0.27333333333333332</v>
+        <v>0.82</v>
       </c>
       <c r="H57">
-        <v>0.27999999999999997</v>
+        <v>0.83999999999999986</v>
       </c>
       <c r="I57">
-        <v>0.28333333333333333</v>
+        <v>0.85</v>
       </c>
       <c r="J57">
-        <v>0.28333333333333333</v>
+        <v>0.85</v>
       </c>
       <c r="K57">
-        <v>0.28666666666666668</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="L57">
-        <v>0.28666666666666668</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="N57">
         <v>3</v>
@@ -8000,37 +9412,37 @@
         <v>0</v>
       </c>
       <c r="B58">
-        <v>0.19999999999999998</v>
+        <v>0.6</v>
       </c>
       <c r="C58">
-        <v>0.22</v>
+        <v>0.66</v>
       </c>
       <c r="D58">
-        <v>0.25666666666666665</v>
+        <v>0.77</v>
       </c>
       <c r="E58">
-        <v>0.27333333333333332</v>
+        <v>0.82</v>
       </c>
       <c r="F58">
-        <v>0.29333333333333333</v>
+        <v>0.88</v>
       </c>
       <c r="G58">
-        <v>0.30333333333333334</v>
+        <v>0.91</v>
       </c>
       <c r="H58">
-        <v>0.31</v>
+        <v>0.92999999999999994</v>
       </c>
       <c r="I58">
-        <v>0.3133333333333333</v>
+        <v>0.94</v>
       </c>
       <c r="J58">
-        <v>0.3133333333333333</v>
+        <v>0.94</v>
       </c>
       <c r="K58">
-        <v>0.3133333333333333</v>
+        <v>0.94</v>
       </c>
       <c r="L58">
-        <v>0.31666666666666665</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
@@ -8039,47 +9451,47 @@
       </c>
       <c r="B60">
         <f>SUM(B56:B58)</f>
-        <v>0.6</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="C60">
         <f t="shared" ref="C60:L60" si="2">SUM(C56:C58)</f>
-        <v>0.66</v>
+        <v>1.98</v>
       </c>
       <c r="D60">
         <f t="shared" si="2"/>
-        <v>0.76333333333333342</v>
+        <v>2.29</v>
       </c>
       <c r="E60">
         <f t="shared" si="2"/>
-        <v>0.83</v>
+        <v>2.4899999999999998</v>
       </c>
       <c r="F60">
         <f t="shared" si="2"/>
-        <v>0.87333333333333341</v>
+        <v>2.62</v>
       </c>
       <c r="G60">
         <f t="shared" si="2"/>
-        <v>0.9</v>
+        <v>2.7</v>
       </c>
       <c r="H60">
         <f t="shared" si="2"/>
-        <v>0.91666666666666674</v>
+        <v>2.75</v>
       </c>
       <c r="I60">
         <f t="shared" si="2"/>
-        <v>0.92666666666666653</v>
+        <v>2.78</v>
       </c>
       <c r="J60">
         <f t="shared" si="2"/>
-        <v>0.92666666666666653</v>
+        <v>2.78</v>
       </c>
       <c r="K60">
         <f t="shared" si="2"/>
-        <v>0.92999999999999994</v>
+        <v>2.79</v>
       </c>
       <c r="L60">
         <f t="shared" si="2"/>
-        <v>0.93333333333333335</v>
+        <v>2.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>